<commit_message>
almos tokay but dependencies need to be reviewed
</commit_message>
<xml_diff>
--- a/OpenWorld/Resources/Items.xlsx
+++ b/OpenWorld/Resources/Items.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="52">
   <si>
     <t>name</t>
   </si>
@@ -162,6 +162,27 @@
   </si>
   <si>
     <t>Warrior,Ranger,Rouge,Acolyte,Slayer</t>
+  </si>
+  <si>
+    <t>Healing potion2</t>
+  </si>
+  <si>
+    <t>Healing potion3</t>
+  </si>
+  <si>
+    <t>Healing potion4</t>
+  </si>
+  <si>
+    <t>Healing potion5</t>
+  </si>
+  <si>
+    <t>Healing potion6</t>
+  </si>
+  <si>
+    <t>Healing potion7</t>
+  </si>
+  <si>
+    <t>Healing potion8</t>
   </si>
 </sst>
 </file>
@@ -431,7 +452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -3985,7 +4006,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4046,25 +4069,165 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C3" s="1"/>
+      <c r="A3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="1">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C4" s="1"/>
+      <c r="A4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="1">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C5" s="1"/>
+      <c r="A5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="1">
+        <v>5</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C6" s="1"/>
+      <c r="A6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="1">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="1"/>
+      <c r="A7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="1"/>
+      <c r="A8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="1">
+        <v>5</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="1"/>
+      <c r="A9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="1">
+        <v>5</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>

</xml_diff>

<commit_message>
parsing of different objects separated for dependency reasons
</commit_message>
<xml_diff>
--- a/OpenWorld/Resources/Items.xlsx
+++ b/OpenWorld/Resources/Items.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="58">
   <si>
     <t>name</t>
   </si>
@@ -183,6 +183,24 @@
   </si>
   <si>
     <t>Healing potion8</t>
+  </si>
+  <si>
+    <t>Light armor2</t>
+  </si>
+  <si>
+    <t>Robes2</t>
+  </si>
+  <si>
+    <t>Heavy armor2</t>
+  </si>
+  <si>
+    <t>Light armor3</t>
+  </si>
+  <si>
+    <t>Robes3</t>
+  </si>
+  <si>
+    <t>Heavy armor3</t>
   </si>
 </sst>
 </file>
@@ -2290,7 +2308,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2397,22 +2417,142 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C5" s="1"/>
+      <c r="A5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>-1</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C6" s="1"/>
+      <c r="A6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="1"/>
+      <c r="A7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>-3</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="1"/>
+      <c r="A8" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>-1</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="1"/>
+      <c r="A9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C10" s="1"/>
+      <c r="A10" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>-3</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
@@ -4006,7 +4146,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
loot added, not yet won from fight
</commit_message>
<xml_diff>
--- a/OpenWorld/Resources/Items.xlsx
+++ b/OpenWorld/Resources/Items.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="66">
   <si>
     <t>name</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>Mage,Acolyte,Ranger,Rouge,Slayer</t>
+  </si>
+  <si>
+    <t>Quilted coat</t>
   </si>
 </sst>
 </file>
@@ -2330,7 +2333,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2668,7 +2671,27 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C15" s="2"/>
+      <c r="A15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C16" s="2"/>

</xml_diff>